<commit_message>
Table 6 data for Jeff
</commit_message>
<xml_diff>
--- a/analysis/D_seats_table_6.xlsx
+++ b/analysis/D_seats_table_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/rdametrics/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E41EF4-CF17-DF42-BD9E-310F1BCA5EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53FB506-AE03-8345-AC5A-D6B134021717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14780" yWindow="3480" windowWidth="28040" windowHeight="21160" xr2:uid="{785D77E5-C29D-0942-9F20-A30D7CD13AEB}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="D_seats_table_6" localSheetId="0">Sheet1!$A$1:$M$22</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{DF30028B-8AE6-7B4B-BA29-ECAD85EB1EF4}" name="D_seats_table_6" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/alecramsay/dev/rdametrics/analysis/D_seats_table_6.csv" comma="1">
+    <textPr sourceFile="/Users/alecramsay/dev/rdametrics/analysis/D_seats_table_6.csv" comma="1">
       <textFields count="13">
         <textField type="text"/>
         <textField/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>A0</t>
   </si>
@@ -549,7 +549,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="M46" sqref="A24:M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,1069 +1462,299 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" t="s">
-        <v>9</v>
-      </c>
-      <c r="L25" t="s">
-        <v>10</v>
-      </c>
-      <c r="M25" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="3">
-        <f>C2-$B2</f>
-        <v>8.0000000000008953E-3</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" ref="D26:M26" si="0">D2-$B2</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.11599999999999966</v>
-      </c>
-      <c r="G26" s="3">
-        <f t="shared" si="0"/>
-        <v>-9.3999999999999417E-2</v>
-      </c>
-      <c r="H26" s="3">
-        <f t="shared" si="0"/>
-        <v>-7.7999999999999403E-2</v>
-      </c>
-      <c r="I26" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.19899999999999984</v>
-      </c>
-      <c r="J26" s="3">
-        <f t="shared" si="0"/>
-        <v>0.16099999999999959</v>
-      </c>
-      <c r="K26" s="3">
-        <f t="shared" si="0"/>
-        <v>0.21300000000000097</v>
-      </c>
-      <c r="L26" s="3">
-        <f t="shared" si="0"/>
-        <v>0.21600000000000108</v>
-      </c>
-      <c r="M26" s="3">
-        <f t="shared" si="0"/>
-        <v>0.21000000000000085</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="3">
-        <f t="shared" ref="C27:M27" si="1">C3-$B3</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <f t="shared" si="1"/>
-        <v>-9.4000000000001194E-2</v>
-      </c>
-      <c r="G27" s="3">
-        <f t="shared" si="1"/>
-        <v>-4.8999999999999488E-2</v>
-      </c>
-      <c r="H27" s="3">
-        <f t="shared" si="1"/>
-        <v>-3.0999999999998806E-2</v>
-      </c>
-      <c r="I27" s="3">
-        <f t="shared" si="1"/>
-        <v>-0.1440000000000019</v>
-      </c>
-      <c r="J27" s="3">
-        <f t="shared" si="1"/>
-        <v>5.6000000000000938E-2</v>
-      </c>
-      <c r="K27" s="3">
-        <f t="shared" si="1"/>
-        <v>0.13599999999999923</v>
-      </c>
-      <c r="L27" s="3">
-        <f t="shared" si="1"/>
-        <v>0.17399999999999949</v>
-      </c>
-      <c r="M27" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19999999999999929</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="3">
-        <f t="shared" ref="C28:M28" si="2">C4-$B4</f>
-        <v>-3.0000000000001137E-3</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="3">
-        <f t="shared" si="2"/>
-        <v>-4.4000000000004036E-2</v>
-      </c>
-      <c r="G28" s="3">
-        <f t="shared" si="2"/>
-        <v>7.9999999999998295E-2</v>
-      </c>
-      <c r="H28" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.4000000000002899E-2</v>
-      </c>
-      <c r="I28" s="3">
-        <f t="shared" si="2"/>
-        <v>-8.2999999999998408E-2</v>
-      </c>
-      <c r="J28" s="3">
-        <f t="shared" si="2"/>
-        <v>-3.0999999999998806E-2</v>
-      </c>
-      <c r="K28" s="3">
-        <f t="shared" si="2"/>
-        <v>-7.0000000000000284E-2</v>
-      </c>
-      <c r="L28" s="3">
-        <f t="shared" si="2"/>
-        <v>-3.0999999999998806E-2</v>
-      </c>
-      <c r="M28" s="3">
-        <f t="shared" si="2"/>
-        <v>6.2999999999995282E-2</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="3">
-        <f t="shared" ref="C29:M29" si="3">C5-$B5</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="3">
-        <f t="shared" si="3"/>
-        <v>1.7999999999998906E-2</v>
-      </c>
-      <c r="G29" s="3">
-        <f t="shared" si="3"/>
-        <v>1.0999999999999233E-2</v>
-      </c>
-      <c r="H29" s="3">
-        <f t="shared" si="3"/>
-        <v>1.1999999999998678E-2</v>
-      </c>
-      <c r="I29" s="3">
-        <f t="shared" si="3"/>
-        <v>2.3999999999999133E-2</v>
-      </c>
-      <c r="J29" s="3">
-        <f t="shared" si="3"/>
-        <v>-4.5000000000001705E-2</v>
-      </c>
-      <c r="K29" s="3">
-        <f t="shared" si="3"/>
-        <v>-0.18400000000000105</v>
-      </c>
-      <c r="L29" s="3">
-        <f t="shared" si="3"/>
-        <v>-0.21200000000000152</v>
-      </c>
-      <c r="M29" s="3">
-        <f t="shared" si="3"/>
-        <v>-0.2110000000000003</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="3">
-        <f t="shared" ref="C30:M30" si="4">C6-$B6</f>
-        <v>-2.0000000000024443E-3</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="3">
-        <f t="shared" si="4"/>
-        <v>-1.8999999999998352E-2</v>
-      </c>
-      <c r="G30" s="3">
-        <f t="shared" si="4"/>
-        <v>0.10499999999999687</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="4"/>
-        <v>5.700000000000216E-2</v>
-      </c>
-      <c r="I30" s="3">
-        <f t="shared" si="4"/>
-        <v>3.0999999999998806E-2</v>
-      </c>
-      <c r="J30" s="3">
-        <f t="shared" si="4"/>
-        <v>-3.8000000000003809E-2</v>
-      </c>
-      <c r="K30" s="3">
-        <f t="shared" si="4"/>
-        <v>-0.10300000000000153</v>
-      </c>
-      <c r="L30" s="3">
-        <f t="shared" si="4"/>
-        <v>-0.15899999999999892</v>
-      </c>
-      <c r="M30" s="3">
-        <f t="shared" si="4"/>
-        <v>-0.20199999999999818</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" ref="C31:M31" si="5">C7-$B7</f>
-        <v>-9.9999999999056399E-4</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="3">
-        <f t="shared" si="5"/>
-        <v>5.0000000000096634E-3</v>
-      </c>
-      <c r="G31" s="3">
-        <f t="shared" si="5"/>
-        <v>-3.9000000000001478E-2</v>
-      </c>
-      <c r="H31" s="3">
-        <f t="shared" si="5"/>
-        <v>9.1000000000008185E-2</v>
-      </c>
-      <c r="I31" s="3">
-        <f t="shared" si="5"/>
-        <v>0.10000000000000853</v>
-      </c>
-      <c r="J31" s="3">
-        <f t="shared" si="5"/>
-        <v>-9.8999999999989541E-2</v>
-      </c>
-      <c r="K31" s="3">
-        <f t="shared" si="5"/>
-        <v>-0.20099999999999341</v>
-      </c>
-      <c r="L31" s="3">
-        <f t="shared" si="5"/>
-        <v>-0.33399999999998897</v>
-      </c>
-      <c r="M31" s="3">
-        <f t="shared" si="5"/>
-        <v>-0.4059999999999917</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="3">
-        <f t="shared" ref="C32:M32" si="6">C8-$B8</f>
-        <v>1.000000000000334E-3</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="3">
-        <f t="shared" si="6"/>
-        <v>3.8000000000000256E-2</v>
-      </c>
-      <c r="G32" s="3">
-        <f t="shared" si="6"/>
-        <v>5.400000000000027E-2</v>
-      </c>
-      <c r="H32" s="3">
-        <f t="shared" si="6"/>
-        <v>5.5000000000000604E-2</v>
-      </c>
-      <c r="I32" s="3">
-        <f t="shared" si="6"/>
-        <v>8.4999999999999964E-2</v>
-      </c>
-      <c r="J32" s="3">
-        <f t="shared" si="6"/>
-        <v>-8.0000000000000071E-3</v>
-      </c>
-      <c r="K32" s="3">
-        <f t="shared" si="6"/>
-        <v>-3.5999999999999588E-2</v>
-      </c>
-      <c r="L32" s="3">
-        <f t="shared" si="6"/>
-        <v>-7.299999999999951E-2</v>
-      </c>
-      <c r="M32" s="3">
-        <f t="shared" si="6"/>
-        <v>-8.0000000000000071E-2</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="3">
-        <f t="shared" ref="C33:M33" si="7">C9-$B9</f>
-        <v>-3.9999999999977831E-3</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="3">
-        <f t="shared" si="7"/>
-        <v>0.10200000000000031</v>
-      </c>
-      <c r="G33" s="3">
-        <f t="shared" si="7"/>
-        <v>3.6000000000001364E-2</v>
-      </c>
-      <c r="H33" s="3">
-        <f t="shared" si="7"/>
-        <v>4.6000000000002927E-2</v>
-      </c>
-      <c r="I33" s="3">
-        <f t="shared" si="7"/>
-        <v>0.18700000000000117</v>
-      </c>
-      <c r="J33" s="3">
-        <f t="shared" si="7"/>
-        <v>-7.9999999999991189E-3</v>
-      </c>
-      <c r="K33" s="3">
-        <f t="shared" si="7"/>
-        <v>4.8000000000001819E-2</v>
-      </c>
-      <c r="L33" s="3">
-        <f t="shared" si="7"/>
-        <v>5.9000000000001052E-2</v>
-      </c>
-      <c r="M33" s="3">
-        <f t="shared" si="7"/>
-        <v>6.0000000000002274E-2</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="3">
-        <f t="shared" ref="C34:M34" si="8">C10-$B10</f>
-        <v>-1.5000000000000568E-2</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="3">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="3">
-        <f t="shared" si="8"/>
-        <v>2.2999999999996135E-2</v>
-      </c>
-      <c r="G34" s="3">
-        <f t="shared" si="8"/>
-        <v>5.4000000000002046E-2</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="8"/>
-        <v>-6.9999999999978968E-3</v>
-      </c>
-      <c r="I34" s="3">
-        <f t="shared" si="8"/>
-        <v>5.4999999999999716E-2</v>
-      </c>
-      <c r="J34" s="3">
-        <f t="shared" si="8"/>
-        <v>0.13700000000000045</v>
-      </c>
-      <c r="K34" s="3">
-        <f t="shared" si="8"/>
-        <v>0.27799999999999869</v>
-      </c>
-      <c r="L34" s="3">
-        <f t="shared" si="8"/>
-        <v>0.32099999999999795</v>
-      </c>
-      <c r="M34" s="3">
-        <f t="shared" si="8"/>
-        <v>0.30700000000000216</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" ref="C35:M35" si="9">C11-$B11</f>
-        <v>3.0000000000001137E-3</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="3">
-        <f t="shared" si="9"/>
-        <v>6.9999999999996732E-3</v>
-      </c>
-      <c r="G35" s="3">
-        <f t="shared" si="9"/>
-        <v>4.9999999999998934E-3</v>
-      </c>
-      <c r="H35" s="3">
-        <f t="shared" si="9"/>
-        <v>-1.1999999999999567E-2</v>
-      </c>
-      <c r="I35" s="3">
-        <f t="shared" si="9"/>
-        <v>-4.9999999999998934E-3</v>
-      </c>
-      <c r="J35" s="3">
-        <f t="shared" si="9"/>
-        <v>-3.0000000000000249E-2</v>
-      </c>
-      <c r="K35" s="3">
-        <f t="shared" si="9"/>
-        <v>-6.0999999999999943E-2</v>
-      </c>
-      <c r="L35" s="3">
-        <f t="shared" si="9"/>
-        <v>-7.3999999999999844E-2</v>
-      </c>
-      <c r="M35" s="3">
-        <f t="shared" si="9"/>
-        <v>-7.8999999999999737E-2</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" ref="C36:M36" si="10">C12-$B12</f>
-        <v>1.699999999999946E-2</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="3">
-        <f t="shared" si="10"/>
-        <v>7.0000000000000284E-2</v>
-      </c>
-      <c r="G36" s="3">
-        <f t="shared" si="10"/>
-        <v>-4.4000000000000483E-2</v>
-      </c>
-      <c r="H36" s="3">
-        <f t="shared" si="10"/>
-        <v>2.8999999999999915E-2</v>
-      </c>
-      <c r="I36" s="3">
-        <f t="shared" si="10"/>
-        <v>9.6999999999997755E-2</v>
-      </c>
-      <c r="J36" s="3">
-        <f t="shared" si="10"/>
-        <v>0.13799999999999812</v>
-      </c>
-      <c r="K36" s="3">
-        <f t="shared" si="10"/>
-        <v>0.27499999999999858</v>
-      </c>
-      <c r="L36" s="3">
-        <f t="shared" si="10"/>
-        <v>0.31499999999999773</v>
-      </c>
-      <c r="M36" s="3">
-        <f t="shared" si="10"/>
-        <v>0.31199999999999761</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" ref="C37:M37" si="11">C13-$B13</f>
-        <v>6.9999999999978968E-3</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="3">
-        <f t="shared" si="11"/>
-        <v>-1.300000000000523E-2</v>
-      </c>
-      <c r="G37" s="3">
-        <f t="shared" si="11"/>
-        <v>1.099999999999568E-2</v>
-      </c>
-      <c r="H37" s="3">
-        <f t="shared" si="11"/>
-        <v>-1.1000000000002785E-2</v>
-      </c>
-      <c r="I37" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="3">
-        <f t="shared" si="11"/>
-        <v>0.15799999999999415</v>
-      </c>
-      <c r="K37" s="3">
-        <f t="shared" si="11"/>
-        <v>0.37800000000000011</v>
-      </c>
-      <c r="L37" s="3">
-        <f t="shared" si="11"/>
-        <v>0.56999999999999318</v>
-      </c>
-      <c r="M37" s="3">
-        <f t="shared" si="11"/>
-        <v>0.62699999999999534</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" ref="C38:M38" si="12">C14-$B14</f>
-        <v>0</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="3">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="3">
-        <f t="shared" si="12"/>
-        <v>6.5999999999998948E-2</v>
-      </c>
-      <c r="G38" s="3">
-        <f t="shared" si="12"/>
-        <v>2.2000000000002018E-2</v>
-      </c>
-      <c r="H38" s="3">
-        <f t="shared" si="12"/>
-        <v>4.2000000000001592E-2</v>
-      </c>
-      <c r="I38" s="3">
-        <f t="shared" si="12"/>
-        <v>0.12100000000000222</v>
-      </c>
-      <c r="J38" s="3">
-        <f t="shared" si="12"/>
-        <v>-3.8999999999997925E-2</v>
-      </c>
-      <c r="K38" s="3">
-        <f t="shared" si="12"/>
-        <v>-0.11199999999999832</v>
-      </c>
-      <c r="L38" s="3">
-        <f t="shared" si="12"/>
-        <v>-0.12399999999999878</v>
-      </c>
-      <c r="M38" s="3">
-        <f t="shared" si="12"/>
-        <v>-0.12000000000000099</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" ref="C39:M39" si="13">C15-$B15</f>
-        <v>5.000000000002558E-3</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="3">
-        <f t="shared" si="13"/>
-        <v>7.0000000000000284E-2</v>
-      </c>
-      <c r="G39" s="3">
-        <f t="shared" si="13"/>
-        <v>4.9999999999997158E-2</v>
-      </c>
-      <c r="H39" s="3">
-        <f t="shared" si="13"/>
-        <v>5.2999999999997272E-2</v>
-      </c>
-      <c r="I39" s="3">
-        <f t="shared" si="13"/>
-        <v>0.13899999999999579</v>
-      </c>
-      <c r="J39" s="3">
-        <f t="shared" si="13"/>
-        <v>4.2000000000001592E-2</v>
-      </c>
-      <c r="K39" s="3">
-        <f t="shared" si="13"/>
-        <v>-2.0000000000024443E-3</v>
-      </c>
-      <c r="L39" s="3">
-        <f t="shared" si="13"/>
-        <v>-9.0000000000003411E-3</v>
-      </c>
-      <c r="M39" s="3">
-        <f t="shared" si="13"/>
-        <v>-1.2000000000000455E-2</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" ref="C40:M40" si="14">C16-$B16</f>
-        <v>-3.0000000000001137E-3</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="3">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="3">
-        <f t="shared" si="14"/>
-        <v>0.25200000000000955</v>
-      </c>
-      <c r="G40" s="3">
-        <f t="shared" si="14"/>
-        <v>1.1000000000009891E-2</v>
-      </c>
-      <c r="H40" s="3">
-        <f t="shared" si="14"/>
-        <v>0.17800000000001148</v>
-      </c>
-      <c r="I40" s="3">
-        <f t="shared" si="14"/>
-        <v>0.44500000000000739</v>
-      </c>
-      <c r="J40" s="3">
-        <f t="shared" si="14"/>
-        <v>-9.2999999999989313E-2</v>
-      </c>
-      <c r="K40" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.18999999999999773</v>
-      </c>
-      <c r="L40" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.18199999999998795</v>
-      </c>
-      <c r="M40" s="3">
-        <f t="shared" si="14"/>
-        <v>5.4000000000002046E-2</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" ref="C41:M41" si="15">C17-$B17</f>
-        <v>2.9999999999992255E-3</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="3">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="3">
-        <f t="shared" si="15"/>
-        <v>-6.5000000000000391E-2</v>
-      </c>
-      <c r="G41" s="3">
-        <f t="shared" si="15"/>
-        <v>-0.12800000000000011</v>
-      </c>
-      <c r="H41" s="3">
-        <f t="shared" si="15"/>
-        <v>-0.14400000000000013</v>
-      </c>
-      <c r="I41" s="3">
-        <f t="shared" si="15"/>
-        <v>-0.2110000000000003</v>
-      </c>
-      <c r="J41" s="3">
-        <f t="shared" si="15"/>
-        <v>4.0999999999999481E-2</v>
-      </c>
-      <c r="K41" s="3">
-        <f t="shared" si="15"/>
-        <v>5.4999999999999716E-2</v>
-      </c>
-      <c r="L41" s="3">
-        <f t="shared" si="15"/>
-        <v>4.0999999999999481E-2</v>
-      </c>
-      <c r="M41" s="3">
-        <f t="shared" si="15"/>
-        <v>3.8999999999999702E-2</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" ref="C42:M42" si="16">C18-$B18</f>
-        <v>1.0000000000012221E-3</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E42" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="3">
-        <f t="shared" si="16"/>
-        <v>3.0000000000001137E-2</v>
-      </c>
-      <c r="G42" s="3">
-        <f t="shared" si="16"/>
-        <v>-2.7999999999998693E-2</v>
-      </c>
-      <c r="H42" s="3">
-        <f t="shared" si="16"/>
-        <v>-6.0000000000002274E-3</v>
-      </c>
-      <c r="I42" s="3">
-        <f t="shared" si="16"/>
-        <v>9.9999999999997868E-3</v>
-      </c>
-      <c r="J42" s="3">
-        <f t="shared" si="16"/>
-        <v>-1.1999999999998678E-2</v>
-      </c>
-      <c r="K42" s="3">
-        <f t="shared" si="16"/>
-        <v>-7.9999999999991189E-3</v>
-      </c>
-      <c r="L42" s="3">
-        <f t="shared" si="16"/>
-        <v>2.1000000000000796E-2</v>
-      </c>
-      <c r="M42" s="3">
-        <f t="shared" si="16"/>
-        <v>3.6000000000001364E-2</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" ref="C43:M43" si="17">C19-$B19</f>
-        <v>4.9999999999954525E-3</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="3">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="3">
-        <f t="shared" si="17"/>
-        <v>-4.8000000000001819E-2</v>
-      </c>
-      <c r="G43" s="3">
-        <f t="shared" si="17"/>
-        <v>0.12399999999999523</v>
-      </c>
-      <c r="H43" s="3">
-        <f t="shared" si="17"/>
-        <v>-1.5000000000000568E-2</v>
-      </c>
-      <c r="I43" s="3">
-        <f t="shared" si="17"/>
-        <v>-3.6999999999999034E-2</v>
-      </c>
-      <c r="J43" s="3">
-        <f t="shared" si="17"/>
-        <v>5.6999999999995055E-2</v>
-      </c>
-      <c r="K43" s="3">
-        <f t="shared" si="17"/>
-        <v>4.8999999999999488E-2</v>
-      </c>
-      <c r="L43" s="3">
-        <f t="shared" si="17"/>
-        <v>0.10599999999999454</v>
-      </c>
-      <c r="M43" s="3">
-        <f t="shared" si="17"/>
-        <v>0.11199999999999477</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" ref="C44:M44" si="18">C20-$B20</f>
-        <v>-4.0000000000000036E-3</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E44" s="3">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="F44" s="3">
-        <f t="shared" si="18"/>
-        <v>5.2000000000000046E-2</v>
-      </c>
-      <c r="G44" s="3">
-        <f t="shared" si="18"/>
-        <v>-7.0000000000001172E-3</v>
-      </c>
-      <c r="H44" s="3">
-        <f t="shared" si="18"/>
-        <v>2.0999999999999908E-2</v>
-      </c>
-      <c r="I44" s="3">
-        <f t="shared" si="18"/>
-        <v>8.4999999999999964E-2</v>
-      </c>
-      <c r="J44" s="3">
-        <f t="shared" si="18"/>
-        <v>-0.11099999999999977</v>
-      </c>
-      <c r="K44" s="3">
-        <f t="shared" si="18"/>
-        <v>-0.22599999999999998</v>
-      </c>
-      <c r="L44" s="3">
-        <f t="shared" si="18"/>
-        <v>-0.24199999999999999</v>
-      </c>
-      <c r="M44" s="3">
-        <f t="shared" si="18"/>
-        <v>-0.23999999999999977</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="3">
-        <f t="shared" ref="C45:M45" si="19">C21-$B21</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="3">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="F45" s="3">
-        <f t="shared" si="19"/>
-        <v>-4.9999999999990052E-3</v>
-      </c>
-      <c r="G45" s="3">
-        <f t="shared" si="19"/>
-        <v>-3.8000000000000256E-2</v>
-      </c>
-      <c r="H45" s="3">
-        <f t="shared" si="19"/>
-        <v>6.0000000000002274E-3</v>
-      </c>
-      <c r="I45" s="3">
-        <f t="shared" si="19"/>
-        <v>-3.2000000000000028E-2</v>
-      </c>
-      <c r="J45" s="3">
-        <f t="shared" si="19"/>
-        <v>-0.14700000000000024</v>
-      </c>
-      <c r="K45" s="3">
-        <f t="shared" si="19"/>
-        <v>-0.26499999999999879</v>
-      </c>
-      <c r="L45" s="3">
-        <f t="shared" si="19"/>
-        <v>-0.29599999999999937</v>
-      </c>
-      <c r="M45" s="3">
-        <f t="shared" si="19"/>
-        <v>-0.29499999999999993</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="3">
-        <f t="shared" ref="C46:M46" si="20">C22-$B22</f>
-        <v>9.0000000000003411E-3</v>
-      </c>
-      <c r="D46" s="3">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="3">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="3">
-        <f t="shared" si="20"/>
-        <v>-0.10099999999999909</v>
-      </c>
-      <c r="G46" s="3">
-        <f t="shared" si="20"/>
-        <v>-0.12199999999999989</v>
-      </c>
-      <c r="H46" s="3">
-        <f t="shared" si="20"/>
-        <v>-5.1000000000001933E-2</v>
-      </c>
-      <c r="I46" s="3">
-        <f t="shared" si="20"/>
-        <v>-0.16700000000000159</v>
-      </c>
-      <c r="J46" s="3">
-        <f t="shared" si="20"/>
-        <v>-8.8000000000000966E-2</v>
-      </c>
-      <c r="K46" s="3">
-        <f t="shared" si="20"/>
-        <v>-0.17399999999999949</v>
-      </c>
-      <c r="L46" s="3">
-        <f t="shared" si="20"/>
-        <v>-0.14200000000000301</v>
-      </c>
-      <c r="M46" s="3">
-        <f t="shared" si="20"/>
-        <v>-0.12199999999999989</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>